<commit_message>
added cols to reflect discrepancies with genus species calls
</commit_message>
<xml_diff>
--- a/supplemental_info/tables/191104_CMS_TableS1.xlsx
+++ b/supplemental_info/tables/191104_CMS_TableS1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amy.kistler/Box Sync/2019_Manuscripts/CMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amy.kistler/code/projects/skeeters/supplemental_info/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="3340" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="191104_CMS_TableS1.csv" sheetId="1" r:id="rId1"/>
@@ -1151,7 +1151,7 @@
     <t> **sex based on visual call from collection agency</t>
   </si>
   <si>
-    <t>‡Habitat type and Population info pulled from California Vectorborne Disease Surveillance System (CalSurv) data for each trap site</t>
+    <t>‡Habitat type and Population = information pulled from California Vectorborne Disease Surveillance System (CalSurv) data for each trap site</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1239,14 +1239,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1529,7 +1529,7 @@
   <dimension ref="A1:N158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H142" activeCellId="2" sqref="I1:J1048576 J135 H142"/>
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added cols to reflect discrepancies among visual, sourmash, and ska with shown genus species calls
</commit_message>
<xml_diff>
--- a/supplemental_info/tables/191104_CMS_TableS1.xlsx
+++ b/supplemental_info/tables/191104_CMS_TableS1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="191104_CMS_TableS1.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="389">
   <si>
     <t>Sequence ID</t>
   </si>
@@ -1152,6 +1152,86 @@
   </si>
   <si>
     <t>‡Habitat type and Population = information pulled from California Vectorborne Disease Surveillance System (CalSurv) data for each trap site</t>
+  </si>
+  <si>
+    <t>Discrepant_genus_species_call</t>
+  </si>
+  <si>
+    <t>Discrepant_method</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Culiseta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incidens</t>
+    </r>
+  </si>
+  <si>
+    <t>visual, sourmash</t>
+  </si>
+  <si>
+    <t>Culex tarsalis</t>
+  </si>
+  <si>
+    <t>visual</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Culex </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tarsalis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Culex </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tarsalis</t>
+    </r>
+  </si>
+  <si>
+    <t>no call</t>
+  </si>
+  <si>
+    <t>no vis data</t>
+  </si>
+  <si>
+    <t>Culiseta inornata</t>
+  </si>
+  <si>
+    <t>missing sample? no sourmash or ska call</t>
+  </si>
+  <si>
+    <t>Culex quinquefasciatus</t>
+  </si>
+  <si>
+    <t>Culex pipiens</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1242,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1176,6 +1256,28 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1214,7 +1316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1249,6 +1351,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N158"/>
+  <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" topLeftCell="B112" zoomScale="101" workbookViewId="0">
+      <selection activeCell="O146" sqref="O146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1652,7 @@
     <col min="14" max="14" width="26.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1591,8 +1695,14 @@
       <c r="N1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1635,8 +1745,10 @@
       <c r="N2" s="3">
         <v>27.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1679,8 +1791,10 @@
       <c r="N3" s="3">
         <v>59.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1723,8 +1837,10 @@
       <c r="N4" s="3">
         <v>88.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1767,8 +1883,10 @@
       <c r="N5" s="3">
         <v>88.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1811,8 +1929,10 @@
       <c r="N6" s="3">
         <v>240.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -1855,8 +1975,10 @@
       <c r="N7" s="3">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1899,8 +2021,10 @@
       <c r="N8" s="3">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1943,8 +2067,10 @@
       <c r="N9" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1987,8 +2113,10 @@
       <c r="N10" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -2031,8 +2159,10 @@
       <c r="N11" s="3">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -2075,8 +2205,10 @@
       <c r="N12" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -2119,8 +2251,10 @@
       <c r="N13" s="3">
         <v>86.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2163,8 +2297,10 @@
       <c r="N14" s="3">
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -2207,8 +2343,14 @@
       <c r="N15" s="3">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -2251,8 +2393,10 @@
       <c r="N16" s="3">
         <v>63.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -2295,8 +2439,10 @@
       <c r="N17" s="3">
         <v>153.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -2339,8 +2485,10 @@
       <c r="N18" s="3">
         <v>73.900000000000006</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>62</v>
       </c>
@@ -2383,8 +2531,10 @@
       <c r="N19" s="3">
         <v>46.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>64</v>
       </c>
@@ -2427,8 +2577,10 @@
       <c r="N20" s="3">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>66</v>
       </c>
@@ -2471,8 +2623,10 @@
       <c r="N21" s="3">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -2515,8 +2669,10 @@
       <c r="N22" s="3">
         <v>32.200000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>70</v>
       </c>
@@ -2559,8 +2715,10 @@
       <c r="N23" s="3">
         <v>27.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -2603,8 +2761,10 @@
       <c r="N24" s="3">
         <v>98.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -2647,8 +2807,10 @@
       <c r="N25" s="3">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -2691,8 +2853,14 @@
       <c r="N26" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="P26" s="16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
@@ -2735,8 +2903,14 @@
       <c r="N27" s="3">
         <v>60.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="P27" s="16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
@@ -2779,8 +2953,10 @@
       <c r="N28" s="3">
         <v>49.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -2823,8 +2999,10 @@
       <c r="N29" s="3">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
@@ -2867,8 +3045,10 @@
       <c r="N30" s="3">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -2911,8 +3091,10 @@
       <c r="N31" s="3">
         <v>273</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>91</v>
       </c>
@@ -2955,8 +3137,10 @@
       <c r="N32" s="3">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>93</v>
       </c>
@@ -2999,8 +3183,10 @@
       <c r="N33" s="3">
         <v>124.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>97</v>
       </c>
@@ -3043,8 +3229,10 @@
       <c r="N34" s="3">
         <v>32.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>99</v>
       </c>
@@ -3087,8 +3275,10 @@
       <c r="N35" s="3">
         <v>56.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
@@ -3131,8 +3321,10 @@
       <c r="N36" s="3">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>103</v>
       </c>
@@ -3175,8 +3367,10 @@
       <c r="N37" s="3">
         <v>36.200000000000003</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>105</v>
       </c>
@@ -3219,8 +3413,10 @@
       <c r="N38" s="3">
         <v>42.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>107</v>
       </c>
@@ -3263,8 +3459,10 @@
       <c r="N39" s="3">
         <v>74.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>109</v>
       </c>
@@ -3307,8 +3505,10 @@
       <c r="N40" s="3">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
@@ -3351,8 +3551,14 @@
       <c r="N41" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="P41" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>114</v>
       </c>
@@ -3395,8 +3601,10 @@
       <c r="N42" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>116</v>
       </c>
@@ -3439,8 +3647,10 @@
       <c r="N43" s="3">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>118</v>
       </c>
@@ -3483,8 +3693,10 @@
       <c r="N44" s="3">
         <v>134</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
@@ -3527,8 +3739,10 @@
       <c r="N45" s="3">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>122</v>
       </c>
@@ -3571,8 +3785,14 @@
       <c r="N46" s="3">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="P46" s="16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>124</v>
       </c>
@@ -3615,8 +3835,10 @@
       <c r="N47" s="3">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>126</v>
       </c>
@@ -3659,8 +3881,10 @@
       <c r="N48" s="3">
         <v>48.4</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>128</v>
       </c>
@@ -3703,8 +3927,10 @@
       <c r="N49" s="3">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>130</v>
       </c>
@@ -3747,8 +3973,10 @@
       <c r="N50" s="3">
         <v>54.4</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>132</v>
       </c>
@@ -3791,8 +4019,10 @@
       <c r="N51" s="3">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>134</v>
       </c>
@@ -3835,8 +4065,10 @@
       <c r="N52" s="3">
         <v>94.3</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>136</v>
       </c>
@@ -3879,8 +4111,10 @@
       <c r="N53" s="3">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>138</v>
       </c>
@@ -3923,8 +4157,10 @@
       <c r="N54" s="3">
         <v>75.599999999999994</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>140</v>
       </c>
@@ -3967,8 +4203,10 @@
       <c r="N55" s="3">
         <v>69.599999999999994</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>142</v>
       </c>
@@ -4011,8 +4249,10 @@
       <c r="N56" s="3">
         <v>34.799999999999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>144</v>
       </c>
@@ -4055,8 +4295,10 @@
       <c r="N57" s="3">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>146</v>
       </c>
@@ -4099,8 +4341,10 @@
       <c r="N58" s="3">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>148</v>
       </c>
@@ -4143,8 +4387,14 @@
       <c r="N59" s="3">
         <v>82.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="P59" s="16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>150</v>
       </c>
@@ -4187,8 +4437,10 @@
       <c r="N60" s="3">
         <v>201</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>152</v>
       </c>
@@ -4225,8 +4477,14 @@
       <c r="N61" s="3">
         <v>66</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="P61" s="16" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>154</v>
       </c>
@@ -4269,8 +4527,10 @@
       <c r="N62" s="3">
         <v>78.400000000000006</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>161</v>
       </c>
@@ -4313,8 +4573,10 @@
       <c r="N63" s="3">
         <v>101.6</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>164</v>
       </c>
@@ -4357,8 +4619,14 @@
       <c r="N64" s="3">
         <v>103.2</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="P64" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>166</v>
       </c>
@@ -4401,8 +4669,10 @@
       <c r="N65" s="3">
         <v>264</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>169</v>
       </c>
@@ -4445,8 +4715,10 @@
       <c r="N66" s="3">
         <v>30.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66" s="16"/>
+      <c r="P66" s="16"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>171</v>
       </c>
@@ -4489,8 +4761,10 @@
       <c r="N67" s="3">
         <v>81.599999999999994</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>176</v>
       </c>
@@ -4533,8 +4807,10 @@
       <c r="N68" s="3">
         <v>62.4</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>179</v>
       </c>
@@ -4577,8 +4853,10 @@
       <c r="N69" s="3">
         <v>54.4</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69" s="16"/>
+      <c r="P69" s="16"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>181</v>
       </c>
@@ -4621,8 +4899,10 @@
       <c r="N70" s="3">
         <v>34.799999999999997</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O70" s="16"/>
+      <c r="P70" s="16"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>183</v>
       </c>
@@ -4665,8 +4945,10 @@
       <c r="N71" s="3">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>185</v>
       </c>
@@ -4709,8 +4991,10 @@
       <c r="N72" s="3">
         <v>45.2</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>187</v>
       </c>
@@ -4753,8 +5037,10 @@
       <c r="N73" s="3">
         <v>138.4</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>189</v>
       </c>
@@ -4797,8 +5083,10 @@
       <c r="N74" s="3">
         <v>32.4</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>191</v>
       </c>
@@ -4841,8 +5129,10 @@
       <c r="N75" s="3">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O75" s="16"/>
+      <c r="P75" s="16"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>193</v>
       </c>
@@ -4885,8 +5175,10 @@
       <c r="N76" s="3">
         <v>135.19999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O76" s="16"/>
+      <c r="P76" s="16"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>197</v>
       </c>
@@ -4929,8 +5221,10 @@
       <c r="N77" s="3">
         <v>260.8</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O77" s="16"/>
+      <c r="P77" s="16"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>199</v>
       </c>
@@ -4973,8 +5267,10 @@
       <c r="N78" s="3">
         <v>148</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O78" s="16"/>
+      <c r="P78" s="16"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>201</v>
       </c>
@@ -5017,8 +5313,10 @@
       <c r="N79" s="3">
         <v>242.4</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O79" s="16"/>
+      <c r="P79" s="16"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>203</v>
       </c>
@@ -5061,8 +5359,10 @@
       <c r="N80" s="3">
         <v>145.6</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O80" s="16"/>
+      <c r="P80" s="16"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>205</v>
       </c>
@@ -5105,8 +5405,10 @@
       <c r="N81" s="3">
         <v>235.2</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O81" s="16"/>
+      <c r="P81" s="16"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>207</v>
       </c>
@@ -5149,8 +5451,10 @@
       <c r="N82" s="3">
         <v>96</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O82" s="16"/>
+      <c r="P82" s="16"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>209</v>
       </c>
@@ -5193,8 +5497,10 @@
       <c r="N83" s="3">
         <v>61.6</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O83" s="16"/>
+      <c r="P83" s="16"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>211</v>
       </c>
@@ -5237,8 +5543,10 @@
       <c r="N84" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O84" s="16"/>
+      <c r="P84" s="16"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>215</v>
       </c>
@@ -5281,8 +5589,10 @@
       <c r="N85" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O85" s="16"/>
+      <c r="P85" s="16"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>217</v>
       </c>
@@ -5325,8 +5635,10 @@
       <c r="N86" s="3">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86" s="16"/>
+      <c r="P86" s="16"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -5369,8 +5681,10 @@
       <c r="N87" s="3">
         <v>50.8</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O87" s="16"/>
+      <c r="P87" s="16"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>221</v>
       </c>
@@ -5413,8 +5727,10 @@
       <c r="N88" s="3">
         <v>36.64</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O88" s="16"/>
+      <c r="P88" s="16"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>223</v>
       </c>
@@ -5457,8 +5773,10 @@
       <c r="N89" s="3">
         <v>296</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O89" s="16"/>
+      <c r="P89" s="16"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>225</v>
       </c>
@@ -5501,8 +5819,10 @@
       <c r="N90" s="3">
         <v>29.12</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O90" s="16"/>
+      <c r="P90" s="16"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>228</v>
       </c>
@@ -5545,8 +5865,10 @@
       <c r="N91" s="3">
         <v>26.96</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O91" s="16"/>
+      <c r="P91" s="16"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>230</v>
       </c>
@@ -5589,8 +5911,10 @@
       <c r="N92" s="3">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O92" s="16"/>
+      <c r="P92" s="16"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>232</v>
       </c>
@@ -5633,8 +5957,10 @@
       <c r="N93" s="3">
         <v>119.2</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O93" s="16"/>
+      <c r="P93" s="16"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>234</v>
       </c>
@@ -5677,8 +6003,10 @@
       <c r="N94" s="3">
         <v>27.44</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O94" s="16"/>
+      <c r="P94" s="16"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>236</v>
       </c>
@@ -5721,8 +6049,10 @@
       <c r="N95" s="3">
         <v>189.6</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O95" s="16"/>
+      <c r="P95" s="16"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>239</v>
       </c>
@@ -5765,8 +6095,10 @@
       <c r="N96" s="3">
         <v>191.2</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O96" s="16"/>
+      <c r="P96" s="16"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>241</v>
       </c>
@@ -5809,8 +6141,10 @@
       <c r="N97" s="3">
         <v>82.4</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O97" s="16"/>
+      <c r="P97" s="16"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>244</v>
       </c>
@@ -5853,8 +6187,10 @@
       <c r="N98" s="3">
         <v>104.8</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O98" s="16"/>
+      <c r="P98" s="16"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>246</v>
       </c>
@@ -5897,8 +6233,10 @@
       <c r="N99" s="3">
         <v>48.4</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O99" s="16"/>
+      <c r="P99" s="16"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>248</v>
       </c>
@@ -5941,8 +6279,10 @@
       <c r="N100" s="3">
         <v>57.2</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O100" s="16"/>
+      <c r="P100" s="16"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>250</v>
       </c>
@@ -5985,8 +6325,10 @@
       <c r="N101" s="3">
         <v>79.599999999999994</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O101" s="16"/>
+      <c r="P101" s="16"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>252</v>
       </c>
@@ -6029,8 +6371,10 @@
       <c r="N102" s="3">
         <v>121.6</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O102" s="16"/>
+      <c r="P102" s="16"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>254</v>
       </c>
@@ -6073,8 +6417,10 @@
       <c r="N103" s="3">
         <v>179.2</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O103" s="16"/>
+      <c r="P103" s="16"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>256</v>
       </c>
@@ -6117,8 +6463,10 @@
       <c r="N104" s="3">
         <v>179.2</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O104" s="16"/>
+      <c r="P104" s="16"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>258</v>
       </c>
@@ -6161,8 +6509,10 @@
       <c r="N105" s="3">
         <v>116.8</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O105" s="16"/>
+      <c r="P105" s="16"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>260</v>
       </c>
@@ -6205,8 +6555,10 @@
       <c r="N106" s="3">
         <v>47.2</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O106" s="16"/>
+      <c r="P106" s="16"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>262</v>
       </c>
@@ -6249,8 +6601,10 @@
       <c r="N107" s="3">
         <v>27.68</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O107" s="16"/>
+      <c r="P107" s="16"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>266</v>
       </c>
@@ -6293,8 +6647,10 @@
       <c r="N108" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O108" s="16"/>
+      <c r="P108" s="16"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>269</v>
       </c>
@@ -6337,8 +6693,10 @@
       <c r="N109" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O109" s="16"/>
+      <c r="P109" s="16"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>272</v>
       </c>
@@ -6381,8 +6739,10 @@
       <c r="N110" s="3">
         <v>39.840000000000003</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O110" s="16"/>
+      <c r="P110" s="16"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>274</v>
       </c>
@@ -6425,8 +6785,10 @@
       <c r="N111" s="3">
         <v>30.32</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O111" s="16"/>
+      <c r="P111" s="16"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>277</v>
       </c>
@@ -6469,8 +6831,10 @@
       <c r="N112" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O112" s="16"/>
+      <c r="P112" s="16"/>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>280</v>
       </c>
@@ -6513,8 +6877,10 @@
       <c r="N113" s="3">
         <v>73.2</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O113" s="16"/>
+      <c r="P113" s="16"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>282</v>
       </c>
@@ -6557,8 +6923,10 @@
       <c r="N114" s="3">
         <v>31.12</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O114" s="16"/>
+      <c r="P114" s="16"/>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>284</v>
       </c>
@@ -6601,8 +6969,10 @@
       <c r="N115" s="3">
         <v>28.72</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O115" s="16"/>
+      <c r="P115" s="16"/>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>286</v>
       </c>
@@ -6645,8 +7015,10 @@
       <c r="N116" s="3">
         <v>31.12</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O116" s="16"/>
+      <c r="P116" s="16"/>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>288</v>
       </c>
@@ -6689,8 +7061,10 @@
       <c r="N117" s="3">
         <v>20.72</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O117" s="16"/>
+      <c r="P117" s="16"/>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>290</v>
       </c>
@@ -6733,8 +7107,10 @@
       <c r="N118" s="3">
         <v>54.4</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O118" s="16"/>
+      <c r="P118" s="16"/>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>292</v>
       </c>
@@ -6777,8 +7153,10 @@
       <c r="N119" s="3">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O119" s="16"/>
+      <c r="P119" s="16"/>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>294</v>
       </c>
@@ -6821,8 +7199,10 @@
       <c r="N120" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O120" s="16"/>
+      <c r="P120" s="16"/>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>296</v>
       </c>
@@ -6865,8 +7245,10 @@
       <c r="N121" s="3">
         <v>74.8</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O121" s="16"/>
+      <c r="P121" s="16"/>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>298</v>
       </c>
@@ -6909,8 +7291,10 @@
       <c r="N122" s="3">
         <v>31.04</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O122" s="16"/>
+      <c r="P122" s="16"/>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -6953,8 +7337,10 @@
       <c r="N123" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O123" s="16"/>
+      <c r="P123" s="16"/>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>302</v>
       </c>
@@ -6997,8 +7383,10 @@
       <c r="N124" s="3">
         <v>69.2</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O124" s="16"/>
+      <c r="P124" s="16"/>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>304</v>
       </c>
@@ -7041,8 +7429,10 @@
       <c r="N125" s="3">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O125" s="16"/>
+      <c r="P125" s="16"/>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>306</v>
       </c>
@@ -7085,8 +7475,10 @@
       <c r="N126" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O126" s="16"/>
+      <c r="P126" s="16"/>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>308</v>
       </c>
@@ -7129,8 +7521,10 @@
       <c r="N127" s="3">
         <v>26.96</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O127" s="16"/>
+      <c r="P127" s="16"/>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>310</v>
       </c>
@@ -7173,8 +7567,10 @@
       <c r="N128" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O128" s="16"/>
+      <c r="P128" s="16"/>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>312</v>
       </c>
@@ -7217,8 +7613,10 @@
       <c r="N129" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O129" s="16"/>
+      <c r="P129" s="16"/>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>314</v>
       </c>
@@ -7261,8 +7659,10 @@
       <c r="N130" s="3">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O130" s="16"/>
+      <c r="P130" s="16"/>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>316</v>
       </c>
@@ -7305,8 +7705,10 @@
       <c r="N131" s="3">
         <v>88.8</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O131" s="16"/>
+      <c r="P131" s="16"/>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>318</v>
       </c>
@@ -7349,8 +7751,10 @@
       <c r="N132" s="3">
         <v>88.8</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O132" s="16"/>
+      <c r="P132" s="16"/>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>320</v>
       </c>
@@ -7393,8 +7797,10 @@
       <c r="N133" s="3">
         <v>70.8</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O133" s="16"/>
+      <c r="P133" s="16"/>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>322</v>
       </c>
@@ -7437,8 +7843,10 @@
       <c r="N134" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O134" s="16"/>
+      <c r="P134" s="16"/>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>324</v>
       </c>
@@ -7481,8 +7889,10 @@
       <c r="N135" s="3">
         <v>37.04</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O135" s="16"/>
+      <c r="P135" s="16"/>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>326</v>
       </c>
@@ -7525,8 +7935,10 @@
       <c r="N136" s="3">
         <v>53.6</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O136" s="16"/>
+      <c r="P136" s="16"/>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>328</v>
       </c>
@@ -7569,8 +7981,10 @@
       <c r="N137" s="3">
         <v>78.400000000000006</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O137" s="16"/>
+      <c r="P137" s="16"/>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>330</v>
       </c>
@@ -7613,8 +8027,10 @@
       <c r="N138" s="3">
         <v>39.520000000000003</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O138" s="16"/>
+      <c r="P138" s="16"/>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>332</v>
       </c>
@@ -7657,8 +8073,10 @@
       <c r="N139" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O139" s="16"/>
+      <c r="P139" s="16"/>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>334</v>
       </c>
@@ -7701,8 +8119,10 @@
       <c r="N140" s="3">
         <v>65.2</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O140" s="16"/>
+      <c r="P140" s="16"/>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>336</v>
       </c>
@@ -7745,8 +8165,10 @@
       <c r="N141" s="3">
         <v>94.4</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O141" s="16"/>
+      <c r="P141" s="16"/>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>338</v>
       </c>
@@ -7789,8 +8211,10 @@
       <c r="N142" s="3">
         <v>48.4</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O142" s="16"/>
+      <c r="P142" s="16"/>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>340</v>
       </c>
@@ -7833,8 +8257,10 @@
       <c r="N143" s="3">
         <v>78.8</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O143" s="16"/>
+      <c r="P143" s="16"/>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>345</v>
       </c>
@@ -7877,8 +8303,10 @@
       <c r="N144" s="3">
         <v>326.39999999999998</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O144" s="16"/>
+      <c r="P144" s="16"/>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>348</v>
       </c>
@@ -7921,8 +8349,10 @@
       <c r="N145" s="3">
         <v>199.2</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O145" s="16"/>
+      <c r="P145" s="16"/>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="s">
         <v>368</v>
       </c>
@@ -7965,8 +8395,14 @@
       <c r="N146" s="11">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O146" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="P146" s="16" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>350</v>
       </c>
@@ -8009,8 +8445,10 @@
       <c r="N147" s="3">
         <v>168.8</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O147" s="16"/>
+      <c r="P147" s="16"/>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>353</v>
       </c>
@@ -8053,8 +8491,10 @@
       <c r="N148" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O148" s="16"/>
+      <c r="P148" s="16"/>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>356</v>
       </c>
@@ -8097,46 +8537,68 @@
       <c r="N149" s="3">
         <v>47.2</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O149" s="16"/>
+      <c r="P149" s="16"/>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O150" s="16"/>
+      <c r="P150" s="16"/>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O151" s="16"/>
+      <c r="P151" s="16"/>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O152" s="16"/>
+      <c r="P152" s="16"/>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O153" s="16"/>
+      <c r="P153" s="16"/>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O154" s="16"/>
+      <c r="P154" s="16"/>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O155" s="16"/>
+      <c r="P155" s="16"/>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O156" s="16"/>
+      <c r="P156" s="16"/>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O157" s="16"/>
+      <c r="P157" s="16"/>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>374</v>
       </c>
+      <c r="O158" s="16"/>
+      <c r="P158" s="16"/>
     </row>
   </sheetData>
   <sortState ref="A2:N148">

</xml_diff>